<commit_message>
Updated excel sheet. Added total number of files corresponding to intents.
</commit_message>
<xml_diff>
--- a/Horn_Intent_Recognition/horn_intents.xlsx
+++ b/Horn_Intent_Recognition/horn_intents.xlsx
@@ -5,22 +5,35 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAY1HYD\Documents\Learning\Research\Horn_Intent_Recognition\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MAY1HYD\Documents\Parking Project\Git-Research\Research-Project\Horn_Intent_Recognition\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8654B15D-96BA-41C3-B3E1-B487D6816BA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57E2DA8-4506-4E90-BB62-0AF74ABCEB70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1082" uniqueCount="545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1087" uniqueCount="547">
   <si>
     <t>filename</t>
   </si>
@@ -1655,6 +1668,12 @@
   </si>
   <si>
     <t>_J_9_S_V.wav</t>
+  </si>
+  <si>
+    <t>Type of intent</t>
+  </si>
+  <si>
+    <t>No. of files</t>
   </si>
 </sst>
 </file>
@@ -1710,10 +1729,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2017,49 +2042,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B541"/>
+  <dimension ref="A1:D541"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.08984375" customWidth="1"/>
     <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="3" max="3" width="22.08984375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2">
+        <f>COUNTIF(B:B, "Warning about a hazard")</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2">
+        <f>COUNTIF(B:B, "Indicating presence")</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2">
+        <f>COUNTIF(B:B, "Frustration or hazard")</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -2067,7 +2123,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -2075,7 +2131,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2083,7 +2139,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2091,7 +2147,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2099,7 +2155,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -2107,7 +2163,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -2115,7 +2171,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -2123,7 +2179,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -2131,7 +2187,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -2139,7 +2195,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -2147,7 +2203,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>19</v>
       </c>

</xml_diff>